<commit_message>
Re-generate CPU summary tables and plots:
* supplementary_table_s5.csv
* CPU time plots

The new tables and plots illustrate that SigProfilerExtractor has much shorter CPU time on HPC-cluster compared to monster2
</commit_message>
<xml_diff>
--- a/output_for_paper/supplementary_table_s5.xlsx
+++ b/output_for_paper/supplementary_table_s5.xlsx
@@ -1469,10 +1469,10 @@
         <v>13</v>
       </c>
       <c r="C77" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D77" t="n">
-        <v>3848239.21</v>
+        <v>2102739.36</v>
       </c>
     </row>
     <row r="78">
@@ -1483,10 +1483,10 @@
         <v>13</v>
       </c>
       <c r="C78" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D78" t="n">
-        <v>3749668.53</v>
+        <v>2107598.81</v>
       </c>
     </row>
     <row r="79">
@@ -1497,10 +1497,10 @@
         <v>13</v>
       </c>
       <c r="C79" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D79" t="n">
-        <v>3949493.73</v>
+        <v>2086986.95</v>
       </c>
     </row>
     <row r="80">
@@ -1511,24 +1511,24 @@
         <v>13</v>
       </c>
       <c r="C80" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D80" t="n">
-        <v>3846206.98</v>
+        <v>2113732.91</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B81" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="C81" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="D81" t="n">
-        <v>3974440.67</v>
+        <v>1694469.415</v>
       </c>
     </row>
     <row r="82">
@@ -1539,10 +1539,10 @@
         <v>17</v>
       </c>
       <c r="C82" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D82" t="n">
-        <v>1694469.415</v>
+        <v>1319799.728</v>
       </c>
     </row>
     <row r="83">
@@ -1553,10 +1553,10 @@
         <v>17</v>
       </c>
       <c r="C83" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D83" t="n">
-        <v>1319799.728</v>
+        <v>1459552.914</v>
       </c>
     </row>
     <row r="84">
@@ -1567,10 +1567,10 @@
         <v>17</v>
       </c>
       <c r="C84" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D84" t="n">
-        <v>1459552.914</v>
+        <v>1414006.838</v>
       </c>
     </row>
     <row r="85">
@@ -1581,24 +1581,24 @@
         <v>17</v>
       </c>
       <c r="C85" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D85" t="n">
-        <v>1414006.838</v>
+        <v>1616929.555</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B86" t="s">
         <v>17</v>
       </c>
       <c r="C86" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="D86" t="n">
-        <v>1616929.555</v>
+        <v>2989747.226</v>
       </c>
     </row>
     <row r="87">
@@ -1609,10 +1609,10 @@
         <v>17</v>
       </c>
       <c r="C87" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D87" t="n">
-        <v>2989747.226</v>
+        <v>3014169.645</v>
       </c>
     </row>
     <row r="88">
@@ -1623,10 +1623,10 @@
         <v>17</v>
       </c>
       <c r="C88" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D88" t="n">
-        <v>3014169.645</v>
+        <v>3007256.781</v>
       </c>
     </row>
     <row r="89">
@@ -1637,10 +1637,10 @@
         <v>17</v>
       </c>
       <c r="C89" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D89" t="n">
-        <v>3007256.781</v>
+        <v>3015428.688</v>
       </c>
     </row>
     <row r="90">
@@ -1651,23 +1651,9 @@
         <v>17</v>
       </c>
       <c r="C90" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D90" t="n">
-        <v>3015428.688</v>
-      </c>
-    </row>
-    <row r="91">
-      <c r="A91" t="s">
-        <v>16</v>
-      </c>
-      <c r="B91" t="s">
-        <v>17</v>
-      </c>
-      <c r="C91" t="s">
-        <v>10</v>
-      </c>
-      <c r="D91" t="n">
         <v>3015978.896</v>
       </c>
     </row>

</xml_diff>

<commit_message>
modified summary code to delete non-useful files in each seed directory
</commit_message>
<xml_diff>
--- a/output_for_paper/supplementary_table_s5.xlsx
+++ b/output_for_paper/supplementary_table_s5.xlsx
@@ -1122,7 +1122,7 @@
         <v>6</v>
       </c>
       <c r="D52" t="n">
-        <v>3302646.823</v>
+        <v>2470313.891</v>
       </c>
     </row>
     <row r="53">
@@ -1136,7 +1136,7 @@
         <v>7</v>
       </c>
       <c r="D53" t="n">
-        <v>3063782.962</v>
+        <v>2256001.79</v>
       </c>
     </row>
     <row r="54">
@@ -1150,7 +1150,7 @@
         <v>8</v>
       </c>
       <c r="D54" t="n">
-        <v>3407795.45</v>
+        <v>1989436.843</v>
       </c>
     </row>
     <row r="55">
@@ -1164,7 +1164,7 @@
         <v>9</v>
       </c>
       <c r="D55" t="n">
-        <v>3161017.217</v>
+        <v>2404490.336</v>
       </c>
     </row>
     <row r="56">
@@ -1178,7 +1178,7 @@
         <v>10</v>
       </c>
       <c r="D56" t="n">
-        <v>4219074.275</v>
+        <v>2387742.679</v>
       </c>
     </row>
     <row r="57">
@@ -1514,7 +1514,7 @@
         <v>9</v>
       </c>
       <c r="D80" t="n">
-        <v>2086986.95</v>
+        <v>3846206.98</v>
       </c>
     </row>
     <row r="81">

</xml_diff>

<commit_message>
Re-generated Supp Tables S4 and S5.
In common_code/summarize_level1_dirs.R, we also uploaded some workarounds to render the embedded list inside of the cell of tibble
</commit_message>
<xml_diff>
--- a/output_for_paper/supplementary_table_s5.xlsx
+++ b/output_for_paper/supplementary_table_s5.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t xml:space="preserve">Data_set</t>
   </si>
@@ -60,6 +60,9 @@
   </si>
   <si>
     <t xml:space="preserve">SBS_set1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SP_narrower_range</t>
   </si>
   <si>
     <t xml:space="preserve">SBS_set2</t>
@@ -1052,7 +1055,7 @@
         <v>6</v>
       </c>
       <c r="D47" t="n">
-        <v>4016281.778</v>
+        <v>2573377.398</v>
       </c>
     </row>
     <row r="48">
@@ -1066,7 +1069,7 @@
         <v>7</v>
       </c>
       <c r="D48" t="n">
-        <v>4245677.486</v>
+        <v>2451739.718</v>
       </c>
     </row>
     <row r="49">
@@ -1080,7 +1083,7 @@
         <v>8</v>
       </c>
       <c r="D49" t="n">
-        <v>4232091.226</v>
+        <v>2529103.88</v>
       </c>
     </row>
     <row r="50">
@@ -1094,7 +1097,7 @@
         <v>9</v>
       </c>
       <c r="D50" t="n">
-        <v>4122607.682</v>
+        <v>2533497.948</v>
       </c>
     </row>
     <row r="51">
@@ -1108,7 +1111,7 @@
         <v>10</v>
       </c>
       <c r="D51" t="n">
-        <v>4233571.47</v>
+        <v>2522122.847</v>
       </c>
     </row>
     <row r="52">
@@ -1122,7 +1125,7 @@
         <v>6</v>
       </c>
       <c r="D52" t="n">
-        <v>2470313.891</v>
+        <v>2500769.117</v>
       </c>
     </row>
     <row r="53">
@@ -1192,7 +1195,7 @@
         <v>6</v>
       </c>
       <c r="D57" t="n">
-        <v>357324.52</v>
+        <v>790904.3</v>
       </c>
     </row>
     <row r="58">
@@ -1206,7 +1209,7 @@
         <v>7</v>
       </c>
       <c r="D58" t="n">
-        <v>393020.23</v>
+        <v>793824.9</v>
       </c>
     </row>
     <row r="59">
@@ -1220,7 +1223,7 @@
         <v>8</v>
       </c>
       <c r="D59" t="n">
-        <v>361345.89</v>
+        <v>791003.05</v>
       </c>
     </row>
     <row r="60">
@@ -1234,7 +1237,7 @@
         <v>9</v>
       </c>
       <c r="D60" t="n">
-        <v>360435.51</v>
+        <v>789803.49</v>
       </c>
     </row>
     <row r="61">
@@ -1248,426 +1251,496 @@
         <v>10</v>
       </c>
       <c r="D61" t="n">
-        <v>359717.25</v>
+        <v>789518.97</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="s">
+        <v>15</v>
+      </c>
+      <c r="B62" t="s">
         <v>16</v>
       </c>
-      <c r="B62" t="s">
-        <v>5</v>
-      </c>
       <c r="C62" t="s">
         <v>6</v>
       </c>
       <c r="D62" t="n">
-        <v>24462112.846</v>
+        <v>357324.52</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="s">
+        <v>15</v>
+      </c>
+      <c r="B63" t="s">
         <v>16</v>
       </c>
-      <c r="B63" t="s">
-        <v>5</v>
-      </c>
       <c r="C63" t="s">
         <v>7</v>
       </c>
       <c r="D63" t="n">
-        <v>23800788.824</v>
+        <v>393020.23</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="s">
+        <v>15</v>
+      </c>
+      <c r="B64" t="s">
         <v>16</v>
       </c>
-      <c r="B64" t="s">
-        <v>5</v>
-      </c>
       <c r="C64" t="s">
         <v>8</v>
       </c>
       <c r="D64" t="n">
-        <v>25439862.31</v>
+        <v>361345.89</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="s">
+        <v>15</v>
+      </c>
+      <c r="B65" t="s">
         <v>16</v>
       </c>
-      <c r="B65" t="s">
-        <v>5</v>
-      </c>
       <c r="C65" t="s">
         <v>9</v>
       </c>
       <c r="D65" t="n">
-        <v>24911450.045</v>
+        <v>360435.51</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="s">
+        <v>15</v>
+      </c>
+      <c r="B66" t="s">
         <v>16</v>
       </c>
-      <c r="B66" t="s">
-        <v>5</v>
-      </c>
       <c r="C66" t="s">
         <v>10</v>
       </c>
       <c r="D66" t="n">
-        <v>25037565.107</v>
+        <v>359717.25</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B67" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="C67" t="s">
         <v>6</v>
       </c>
       <c r="D67" t="n">
-        <v>6397205.75</v>
+        <v>24462112.846</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B68" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="C68" t="s">
         <v>7</v>
       </c>
       <c r="D68" t="n">
-        <v>5310002.954</v>
+        <v>23800788.824</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B69" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="C69" t="s">
         <v>8</v>
       </c>
       <c r="D69" t="n">
-        <v>5603919.865</v>
+        <v>25439862.31</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B70" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="C70" t="s">
         <v>9</v>
       </c>
       <c r="D70" t="n">
-        <v>6500565.178</v>
+        <v>24911450.045</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B71" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="C71" t="s">
         <v>10</v>
       </c>
       <c r="D71" t="n">
-        <v>5898554.229</v>
+        <v>25037565.107</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B72" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C72" t="s">
         <v>6</v>
       </c>
       <c r="D72" t="n">
-        <v>1538994.096</v>
+        <v>6397205.75</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B73" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C73" t="s">
         <v>7</v>
       </c>
       <c r="D73" t="n">
-        <v>1656785.884</v>
+        <v>5310002.954</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B74" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C74" t="s">
         <v>8</v>
       </c>
       <c r="D74" t="n">
-        <v>1569906.974</v>
+        <v>5603919.865</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B75" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C75" t="s">
         <v>9</v>
       </c>
       <c r="D75" t="n">
-        <v>1390289.565</v>
+        <v>6500565.178</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B76" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C76" t="s">
         <v>10</v>
       </c>
       <c r="D76" t="n">
-        <v>1442116.337</v>
+        <v>5898554.229</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B77" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C77" t="s">
         <v>6</v>
       </c>
       <c r="D77" t="n">
-        <v>2102332.48</v>
+        <v>1538994.096</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B78" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C78" t="s">
         <v>7</v>
       </c>
       <c r="D78" t="n">
-        <v>2102739.36</v>
+        <v>1656785.884</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B79" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C79" t="s">
         <v>8</v>
       </c>
       <c r="D79" t="n">
-        <v>2107598.81</v>
+        <v>1569906.974</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B80" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C80" t="s">
         <v>9</v>
       </c>
       <c r="D80" t="n">
-        <v>3846206.98</v>
+        <v>1390289.565</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B81" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C81" t="s">
         <v>10</v>
       </c>
       <c r="D81" t="n">
-        <v>2113732.91</v>
+        <v>1442116.337</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B82" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C82" t="s">
         <v>6</v>
       </c>
       <c r="D82" t="n">
-        <v>1694469.415</v>
+        <v>2102332.48</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B83" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C83" t="s">
         <v>7</v>
       </c>
       <c r="D83" t="n">
-        <v>1319799.728</v>
+        <v>2102739.36</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B84" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C84" t="s">
         <v>8</v>
       </c>
       <c r="D84" t="n">
-        <v>1459552.914</v>
+        <v>2107598.81</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B85" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C85" t="s">
         <v>9</v>
       </c>
       <c r="D85" t="n">
-        <v>1414006.838</v>
+        <v>2086986.95</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B86" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C86" t="s">
         <v>10</v>
       </c>
       <c r="D86" t="n">
-        <v>1616929.555</v>
+        <v>2113732.91</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B87" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C87" t="s">
         <v>6</v>
       </c>
       <c r="D87" t="n">
-        <v>2989747.226</v>
+        <v>1322527.022</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B88" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C88" t="s">
         <v>7</v>
       </c>
       <c r="D88" t="n">
-        <v>3014169.645</v>
+        <v>1319799.728</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B89" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C89" t="s">
         <v>8</v>
       </c>
       <c r="D89" t="n">
-        <v>3007256.781</v>
+        <v>1329515.059</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B90" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C90" t="s">
         <v>9</v>
       </c>
       <c r="D90" t="n">
-        <v>3015428.688</v>
+        <v>1320033.22</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B91" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C91" t="s">
         <v>10</v>
       </c>
       <c r="D91" t="n">
+        <v>1323129.048</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="s">
+        <v>17</v>
+      </c>
+      <c r="B92" t="s">
+        <v>18</v>
+      </c>
+      <c r="C92" t="s">
+        <v>6</v>
+      </c>
+      <c r="D92" t="n">
+        <v>2989747.226</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="s">
+        <v>17</v>
+      </c>
+      <c r="B93" t="s">
+        <v>18</v>
+      </c>
+      <c r="C93" t="s">
+        <v>7</v>
+      </c>
+      <c r="D93" t="n">
+        <v>3014169.645</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="s">
+        <v>17</v>
+      </c>
+      <c r="B94" t="s">
+        <v>18</v>
+      </c>
+      <c r="C94" t="s">
+        <v>8</v>
+      </c>
+      <c r="D94" t="n">
+        <v>3007256.781</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="s">
+        <v>17</v>
+      </c>
+      <c r="B95" t="s">
+        <v>18</v>
+      </c>
+      <c r="C95" t="s">
+        <v>9</v>
+      </c>
+      <c r="D95" t="n">
+        <v>3015428.688</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="s">
+        <v>17</v>
+      </c>
+      <c r="B96" t="s">
+        <v>18</v>
+      </c>
+      <c r="C96" t="s">
+        <v>10</v>
+      </c>
+      <c r="D96" t="n">
         <v>3015978.896</v>
       </c>
     </row>

</xml_diff>